<commit_message>
Fix layout and vertical text
</commit_message>
<xml_diff>
--- a/TestPWA/wwwroot/checklist/BPS_1020.xlsx
+++ b/TestPWA/wwwroot/checklist/BPS_1020.xlsx
@@ -1032,7 +1032,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="29">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1079,9 +1079,6 @@
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="10" applyBorder="1" xfId="0">
       <alignment horizontal="center" wrapText="1" textRotation="90"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" borderId="10" applyBorder="1" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="4" applyFill="1" borderId="11" applyBorder="1" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1123,8 +1120,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
@@ -1158,7 +1155,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A3:K62"/>
+  <dimension ref="A3:J62"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1174,11 +1171,10 @@
     <col min="8" max="8" width="4" customWidth="1"/>
     <col min="9" max="9" width="4" customWidth="1"/>
     <col min="10" max="10" width="4" customWidth="1"/>
-    <col min="11" max="11" width="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="28" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1196,8 +1192,7 @@
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7">
       <c r="A7" s="6" t="s">
@@ -1213,8 +1208,7 @@
       <c r="G7" s="9"/>
       <c r="H7" s="9"/>
       <c r="I7" s="9"/>
-      <c r="J7" s="9"/>
-      <c r="K7" s="10"/>
+      <c r="J7" s="10"/>
     </row>
     <row r="8">
       <c r="A8" s="11" t="s">
@@ -1231,7 +1225,6 @@
       <c r="H8" s="14"/>
       <c r="I8" s="14"/>
       <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
     </row>
     <row r="9">
       <c r="A9" s="15" t="s">
@@ -1254,10 +1247,9 @@
       <c r="J9" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K9" s="20"/>
     </row>
     <row r="10">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="9"/>
@@ -1268,11 +1260,10 @@
       <c r="G10" s="9"/>
       <c r="H10" s="9"/>
       <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
-      <c r="K10" s="22"/>
+      <c r="J10" s="21"/>
     </row>
     <row r="11">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="16"/>
@@ -1283,13 +1274,12 @@
       <c r="G11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="24"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23"/>
     </row>
     <row r="12">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="16"/>
@@ -1300,13 +1290,12 @@
       <c r="G12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="24"/>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23"/>
     </row>
     <row r="13">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="16"/>
@@ -1317,13 +1306,12 @@
       <c r="G13" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="H13" s="25"/>
-      <c r="I13" s="25"/>
-      <c r="J13" s="25"/>
-      <c r="K13" s="25"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
     </row>
     <row r="14">
-      <c r="A14" s="23" t="s">
+      <c r="A14" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="16"/>
@@ -1334,13 +1322,12 @@
       <c r="G14" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H14" s="25"/>
-      <c r="I14" s="25"/>
-      <c r="J14" s="25"/>
-      <c r="K14" s="25"/>
+      <c r="H14" s="24"/>
+      <c r="I14" s="24"/>
+      <c r="J14" s="24"/>
     </row>
     <row r="15">
-      <c r="A15" s="23" t="s">
+      <c r="A15" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="16"/>
@@ -1351,13 +1338,12 @@
       <c r="G15" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="H15" s="25"/>
-      <c r="I15" s="25"/>
-      <c r="J15" s="25"/>
-      <c r="K15" s="25"/>
+      <c r="H15" s="24"/>
+      <c r="I15" s="24"/>
+      <c r="J15" s="24"/>
     </row>
     <row r="16">
-      <c r="A16" s="23" t="s">
+      <c r="A16" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B16" s="16"/>
@@ -1368,13 +1354,12 @@
       <c r="G16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="H16" s="25"/>
-      <c r="I16" s="25"/>
-      <c r="J16" s="25"/>
-      <c r="K16" s="25"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
     </row>
     <row r="17">
-      <c r="A17" s="23" t="s">
+      <c r="A17" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B17" s="16"/>
@@ -1385,13 +1370,12 @@
       <c r="G17" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="25"/>
-      <c r="I17" s="25"/>
-      <c r="J17" s="25"/>
-      <c r="K17" s="25"/>
+      <c r="H17" s="24"/>
+      <c r="I17" s="24"/>
+      <c r="J17" s="24"/>
     </row>
     <row r="18">
-      <c r="A18" s="23" t="s">
+      <c r="A18" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B18" s="16"/>
@@ -1402,13 +1386,12 @@
       <c r="G18" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="H18" s="25"/>
-      <c r="I18" s="25"/>
-      <c r="J18" s="25"/>
-      <c r="K18" s="25"/>
+      <c r="H18" s="24"/>
+      <c r="I18" s="24"/>
+      <c r="J18" s="24"/>
     </row>
     <row r="19">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="22" t="s">
         <v>29</v>
       </c>
       <c r="B19" s="16"/>
@@ -1419,13 +1402,12 @@
       <c r="G19" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H19" s="25"/>
-      <c r="I19" s="25"/>
-      <c r="J19" s="25"/>
-      <c r="K19" s="25"/>
+      <c r="H19" s="24"/>
+      <c r="I19" s="24"/>
+      <c r="J19" s="24"/>
     </row>
     <row r="20">
-      <c r="A20" s="23" t="s">
+      <c r="A20" s="22" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="16"/>
@@ -1436,13 +1418,12 @@
       <c r="G20" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="H20" s="25"/>
-      <c r="I20" s="25"/>
-      <c r="J20" s="25"/>
-      <c r="K20" s="25"/>
+      <c r="H20" s="24"/>
+      <c r="I20" s="24"/>
+      <c r="J20" s="24"/>
     </row>
     <row r="21">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="22" t="s">
         <v>33</v>
       </c>
       <c r="B21" s="16"/>
@@ -1453,13 +1434,12 @@
       <c r="G21" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="H21" s="25"/>
-      <c r="I21" s="25"/>
-      <c r="J21" s="25"/>
-      <c r="K21" s="25"/>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="24"/>
     </row>
     <row r="22">
-      <c r="A22" s="23" t="s">
+      <c r="A22" s="22" t="s">
         <v>35</v>
       </c>
       <c r="B22" s="16"/>
@@ -1470,10 +1450,9 @@
       <c r="G22" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H22" s="25"/>
-      <c r="I22" s="25"/>
-      <c r="J22" s="25"/>
-      <c r="K22" s="25"/>
+      <c r="H22" s="24"/>
+      <c r="I22" s="24"/>
+      <c r="J22" s="24"/>
     </row>
     <row r="23">
       <c r="A23" s="17"/>
@@ -1490,7 +1469,7 @@
       <c r="A26" s="17"/>
     </row>
     <row r="27">
-      <c r="A27" s="21" t="s">
+      <c r="A27" s="20" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="9"/>
@@ -1501,18 +1480,17 @@
       <c r="G27" s="9"/>
       <c r="H27" s="9"/>
       <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="22"/>
+      <c r="J27" s="21"/>
     </row>
     <row r="28">
-      <c r="A28" s="26" t="s">
+      <c r="A28" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
-      <c r="D28" s="27"/>
-      <c r="E28" s="27"/>
-      <c r="F28" s="27"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
       <c r="G28" s="19" t="s">
         <v>8</v>
       </c>
@@ -1525,10 +1503,9 @@
       <c r="J28" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K28" s="20"/>
     </row>
     <row r="29">
-      <c r="A29" s="23" t="s">
+      <c r="A29" s="22" t="s">
         <v>39</v>
       </c>
       <c r="B29" s="16"/>
@@ -1539,13 +1516,12 @@
       <c r="G29" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H29" s="25"/>
-      <c r="I29" s="25"/>
-      <c r="J29" s="25"/>
-      <c r="K29" s="25"/>
+      <c r="H29" s="24"/>
+      <c r="I29" s="24"/>
+      <c r="J29" s="24"/>
     </row>
     <row r="30">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="22" t="s">
         <v>40</v>
       </c>
       <c r="B30" s="16"/>
@@ -1556,13 +1532,12 @@
       <c r="G30" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="H30" s="25"/>
-      <c r="I30" s="25"/>
-      <c r="J30" s="25"/>
-      <c r="K30" s="25"/>
+      <c r="H30" s="24"/>
+      <c r="I30" s="24"/>
+      <c r="J30" s="24"/>
     </row>
     <row r="31">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="22" t="s">
         <v>42</v>
       </c>
       <c r="B31" s="16"/>
@@ -1573,13 +1548,12 @@
       <c r="G31" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H31" s="25"/>
-      <c r="I31" s="25"/>
-      <c r="J31" s="25"/>
-      <c r="K31" s="25"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="24"/>
+      <c r="J31" s="24"/>
     </row>
     <row r="32">
-      <c r="A32" s="23" t="s">
+      <c r="A32" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B32" s="16"/>
@@ -1590,10 +1564,9 @@
       <c r="G32" s="15" t="s">
         <v>44</v>
       </c>
-      <c r="H32" s="25"/>
-      <c r="I32" s="25"/>
-      <c r="J32" s="25"/>
-      <c r="K32" s="25"/>
+      <c r="H32" s="24"/>
+      <c r="I32" s="24"/>
+      <c r="J32" s="24"/>
     </row>
     <row r="33">
       <c r="A33" s="17"/>
@@ -1610,7 +1583,7 @@
       <c r="A36" s="17"/>
     </row>
     <row r="37">
-      <c r="A37" s="21" t="s">
+      <c r="A37" s="20" t="s">
         <v>45</v>
       </c>
       <c r="B37" s="9"/>
@@ -1621,18 +1594,17 @@
       <c r="G37" s="9"/>
       <c r="H37" s="9"/>
       <c r="I37" s="9"/>
-      <c r="J37" s="9"/>
-      <c r="K37" s="22"/>
+      <c r="J37" s="21"/>
     </row>
     <row r="38">
-      <c r="A38" s="26" t="s">
+      <c r="A38" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B38" s="27"/>
-      <c r="C38" s="27"/>
-      <c r="D38" s="27"/>
-      <c r="E38" s="27"/>
-      <c r="F38" s="27"/>
+      <c r="B38" s="26"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="26"/>
+      <c r="E38" s="26"/>
+      <c r="F38" s="26"/>
       <c r="G38" s="19" t="s">
         <v>8</v>
       </c>
@@ -1645,10 +1617,9 @@
       <c r="J38" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="K38" s="20"/>
     </row>
     <row r="40">
-      <c r="A40" s="23" t="s">
+      <c r="A40" s="22" t="s">
         <v>46</v>
       </c>
       <c r="B40" s="16"/>
@@ -1659,13 +1630,12 @@
       <c r="G40" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H40" s="25"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="25"/>
-      <c r="K40" s="25"/>
+      <c r="H40" s="24"/>
+      <c r="I40" s="24"/>
+      <c r="J40" s="24"/>
     </row>
     <row r="41">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="22" t="s">
         <v>47</v>
       </c>
       <c r="B41" s="16"/>
@@ -1676,13 +1646,12 @@
       <c r="G41" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="H41" s="25"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="25"/>
-      <c r="K41" s="25"/>
+      <c r="H41" s="24"/>
+      <c r="I41" s="24"/>
+      <c r="J41" s="24"/>
     </row>
     <row r="42">
-      <c r="A42" s="23" t="s">
+      <c r="A42" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B42" s="16"/>
@@ -1693,13 +1662,12 @@
       <c r="G42" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="H42" s="25"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="25"/>
-      <c r="K42" s="25"/>
+      <c r="H42" s="24"/>
+      <c r="I42" s="24"/>
+      <c r="J42" s="24"/>
     </row>
     <row r="43">
-      <c r="A43" s="23" t="s">
+      <c r="A43" s="22" t="s">
         <v>51</v>
       </c>
       <c r="B43" s="16"/>
@@ -1710,13 +1678,12 @@
       <c r="G43" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="H43" s="25"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="25"/>
-      <c r="K43" s="25"/>
+      <c r="H43" s="24"/>
+      <c r="I43" s="24"/>
+      <c r="J43" s="24"/>
     </row>
     <row r="44">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="22" t="s">
         <v>52</v>
       </c>
       <c r="B44" s="16"/>
@@ -1727,13 +1694,12 @@
       <c r="G44" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="H44" s="25"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="25"/>
-      <c r="K44" s="25"/>
+      <c r="H44" s="24"/>
+      <c r="I44" s="24"/>
+      <c r="J44" s="24"/>
     </row>
     <row r="45">
-      <c r="A45" s="23" t="s">
+      <c r="A45" s="22" t="s">
         <v>54</v>
       </c>
       <c r="B45" s="16"/>
@@ -1744,10 +1710,9 @@
       <c r="G45" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H45" s="25"/>
-      <c r="I45" s="25"/>
-      <c r="J45" s="25"/>
-      <c r="K45" s="25"/>
+      <c r="H45" s="24"/>
+      <c r="I45" s="24"/>
+      <c r="J45" s="24"/>
     </row>
     <row r="46">
       <c r="A46" s="17"/>
@@ -1764,7 +1729,7 @@
       <c r="A49" s="17"/>
     </row>
     <row r="50">
-      <c r="A50" s="21" t="s">
+      <c r="A50" s="20" t="s">
         <v>56</v>
       </c>
       <c r="B50" s="9"/>
@@ -1775,17 +1740,16 @@
       <c r="G50" s="9"/>
       <c r="H50" s="9"/>
       <c r="I50" s="9"/>
-      <c r="J50" s="9"/>
-      <c r="K50" s="22"/>
+      <c r="J50" s="21"/>
     </row>
     <row r="51">
-      <c r="A51" s="28" t="s">
+      <c r="A51" s="27" t="s">
         <v>57</v>
       </c>
       <c r="B51" s="16"/>
       <c r="C51" s="16"/>
       <c r="D51" s="16"/>
-      <c r="E51" s="28" t="s">
+      <c r="E51" s="27" t="s">
         <v>58</v>
       </c>
       <c r="F51" s="16"/>
@@ -1797,16 +1761,15 @@
         <v>60</v>
       </c>
       <c r="J51" s="16"/>
-      <c r="K51" s="20"/>
     </row>
     <row r="52">
-      <c r="A52" s="23" t="s">
+      <c r="A52" s="22" t="s">
         <v>61</v>
       </c>
       <c r="B52" s="16"/>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
-      <c r="E52" s="23" t="s">
+      <c r="E52" s="22" t="s">
         <v>62</v>
       </c>
       <c r="F52" s="16"/>
@@ -1818,16 +1781,15 @@
         <v>64</v>
       </c>
       <c r="J52" s="16"/>
-      <c r="K52" s="20"/>
     </row>
     <row r="53">
-      <c r="A53" s="23" t="s">
+      <c r="A53" s="22" t="s">
         <v>65</v>
       </c>
       <c r="B53" s="16"/>
       <c r="C53" s="16"/>
       <c r="D53" s="16"/>
-      <c r="E53" s="23" t="s">
+      <c r="E53" s="22" t="s">
         <v>66</v>
       </c>
       <c r="F53" s="16"/>
@@ -1839,16 +1801,15 @@
         <v>68</v>
       </c>
       <c r="J53" s="16"/>
-      <c r="K53" s="20"/>
     </row>
     <row r="54">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="22" t="s">
         <v>69</v>
       </c>
       <c r="B54" s="16"/>
       <c r="C54" s="16"/>
       <c r="D54" s="16"/>
-      <c r="E54" s="23" t="s">
+      <c r="E54" s="22" t="s">
         <v>70</v>
       </c>
       <c r="F54" s="16"/>
@@ -1860,16 +1821,15 @@
         <v>71</v>
       </c>
       <c r="J54" s="16"/>
-      <c r="K54" s="20"/>
     </row>
     <row r="55">
-      <c r="A55" s="23" t="s">
+      <c r="A55" s="22" t="s">
         <v>72</v>
       </c>
       <c r="B55" s="16"/>
       <c r="C55" s="16"/>
       <c r="D55" s="16"/>
-      <c r="E55" s="23" t="s">
+      <c r="E55" s="22" t="s">
         <v>73</v>
       </c>
       <c r="F55" s="16"/>
@@ -1881,16 +1841,15 @@
         <v>74</v>
       </c>
       <c r="J55" s="16"/>
-      <c r="K55" s="20"/>
     </row>
     <row r="56">
-      <c r="A56" s="23" t="s">
+      <c r="A56" s="22" t="s">
         <v>75</v>
       </c>
       <c r="B56" s="16"/>
       <c r="C56" s="16"/>
       <c r="D56" s="16"/>
-      <c r="E56" s="23" t="s">
+      <c r="E56" s="22" t="s">
         <v>76</v>
       </c>
       <c r="F56" s="16"/>
@@ -1902,16 +1861,15 @@
         <v>77</v>
       </c>
       <c r="J56" s="16"/>
-      <c r="K56" s="20"/>
     </row>
     <row r="57">
-      <c r="A57" s="23" t="s">
+      <c r="A57" s="22" t="s">
         <v>78</v>
       </c>
       <c r="B57" s="16"/>
       <c r="C57" s="16"/>
       <c r="D57" s="16"/>
-      <c r="E57" s="23" t="s">
+      <c r="E57" s="22" t="s">
         <v>79</v>
       </c>
       <c r="F57" s="16"/>
@@ -1923,16 +1881,15 @@
         <v>80</v>
       </c>
       <c r="J57" s="16"/>
-      <c r="K57" s="20"/>
     </row>
     <row r="58">
-      <c r="A58" s="23" t="s">
+      <c r="A58" s="22" t="s">
         <v>81</v>
       </c>
       <c r="B58" s="16"/>
       <c r="C58" s="16"/>
       <c r="D58" s="16"/>
-      <c r="E58" s="23" t="s">
+      <c r="E58" s="22" t="s">
         <v>82</v>
       </c>
       <c r="F58" s="16"/>
@@ -1944,16 +1901,15 @@
         <v>83</v>
       </c>
       <c r="J58" s="16"/>
-      <c r="K58" s="20"/>
     </row>
     <row r="59">
-      <c r="A59" s="23" t="s">
+      <c r="A59" s="22" t="s">
         <v>84</v>
       </c>
       <c r="B59" s="16"/>
       <c r="C59" s="16"/>
       <c r="D59" s="16"/>
-      <c r="E59" s="23" t="s">
+      <c r="E59" s="22" t="s">
         <v>85</v>
       </c>
       <c r="F59" s="16"/>
@@ -1965,7 +1921,6 @@
         <v>86</v>
       </c>
       <c r="J59" s="16"/>
-      <c r="K59" s="20"/>
     </row>
     <row r="60">
       <c r="A60" s="17"/>
@@ -1980,11 +1935,11 @@
     </row>
   </sheetData>
   <mergeCells>
-    <mergeCell ref="D6:K6"/>
-    <mergeCell ref="D7:K7"/>
-    <mergeCell ref="D8:K8"/>
+    <mergeCell ref="D6:J6"/>
+    <mergeCell ref="D7:J7"/>
+    <mergeCell ref="D8:J8"/>
     <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A10:K10"/>
+    <mergeCell ref="A10:J10"/>
     <mergeCell ref="A11:F11"/>
     <mergeCell ref="A12:F12"/>
     <mergeCell ref="A13:F13"/>
@@ -1997,21 +1952,21 @@
     <mergeCell ref="A20:F20"/>
     <mergeCell ref="A21:F21"/>
     <mergeCell ref="A22:F22"/>
-    <mergeCell ref="A23:K23"/>
-    <mergeCell ref="A24:K24"/>
-    <mergeCell ref="A25:K25"/>
-    <mergeCell ref="A26:K26"/>
-    <mergeCell ref="A27:K27"/>
+    <mergeCell ref="A23:J23"/>
+    <mergeCell ref="A24:J24"/>
+    <mergeCell ref="A25:J25"/>
+    <mergeCell ref="A26:J26"/>
+    <mergeCell ref="A27:J27"/>
     <mergeCell ref="A28:F28"/>
     <mergeCell ref="A29:F29"/>
     <mergeCell ref="A30:F30"/>
     <mergeCell ref="A31:F31"/>
     <mergeCell ref="A32:F32"/>
-    <mergeCell ref="A33:K33"/>
-    <mergeCell ref="A34:K34"/>
-    <mergeCell ref="A35:K35"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A37:K37"/>
+    <mergeCell ref="A33:J33"/>
+    <mergeCell ref="A34:J34"/>
+    <mergeCell ref="A35:J35"/>
+    <mergeCell ref="A36:J36"/>
+    <mergeCell ref="A37:J37"/>
     <mergeCell ref="A38:F38"/>
     <mergeCell ref="A40:F40"/>
     <mergeCell ref="A41:F41"/>
@@ -2019,11 +1974,11 @@
     <mergeCell ref="A43:F43"/>
     <mergeCell ref="A44:F44"/>
     <mergeCell ref="A45:F45"/>
-    <mergeCell ref="A46:K46"/>
-    <mergeCell ref="A47:K47"/>
-    <mergeCell ref="A48:K48"/>
-    <mergeCell ref="A49:K49"/>
-    <mergeCell ref="A50:K50"/>
+    <mergeCell ref="A46:J46"/>
+    <mergeCell ref="A47:J47"/>
+    <mergeCell ref="A48:J48"/>
+    <mergeCell ref="A49:J49"/>
+    <mergeCell ref="A50:J50"/>
     <mergeCell ref="A51:D51"/>
     <mergeCell ref="E51:F51"/>
     <mergeCell ref="G51:H51"/>
@@ -2060,9 +2015,9 @@
     <mergeCell ref="E59:F59"/>
     <mergeCell ref="G59:H59"/>
     <mergeCell ref="I59:J59"/>
-    <mergeCell ref="A60:K60"/>
-    <mergeCell ref="A61:K61"/>
-    <mergeCell ref="A62:K62"/>
+    <mergeCell ref="A60:J60"/>
+    <mergeCell ref="A61:J61"/>
+    <mergeCell ref="A62:J62"/>
     <mergeCell ref="A3:E4"/>
   </mergeCells>
   <headerFooter/>

</xml_diff>